<commit_message>
Update level one flux parsing to account for 01 July 2021 raise
</commit_message>
<xml_diff>
--- a/metadata/flux_metadata_level1_15min_July2021.xlsx
+++ b/metadata/flux_metadata_level1_15min_July2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00F8B81-4B0E-0D4A-B849-CF83852D555E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA8F56-E804-4F46-9990-4CBA4740245A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38340" yWindow="-10540" windowWidth="28520" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46860" yWindow="-10580" windowWidth="20000" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -707,10 +707,10 @@
   <dimension ref="A1:M1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>